<commit_message>
Update weight along till dpi 11
</commit_message>
<xml_diff>
--- a/data_raw/NMRIMarch2018/NMRI_Mäuse.xlsx
+++ b/data_raw/NMRIMarch2018/NMRI_Mäuse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivim\Desktop\WiSE1718\Parasitologie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vivim\Desktop\Bachelor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52192029-16DA-4EE6-8002-0C853A218771}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDC3EFE-6509-4979-9DD5-7C4A83659375}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{66AFA6B0-710C-4709-A9F7-0014DEAC4993}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="381">
   <si>
     <t>mouse-ID</t>
   </si>
@@ -919,6 +919,255 @@
   </si>
   <si>
     <t>2.81</t>
+  </si>
+  <si>
+    <t>37.1</t>
+  </si>
+  <si>
+    <t>39.5</t>
+  </si>
+  <si>
+    <t>38.5</t>
+  </si>
+  <si>
+    <t>42.9</t>
+  </si>
+  <si>
+    <t>36.5</t>
+  </si>
+  <si>
+    <t>34.1</t>
+  </si>
+  <si>
+    <t>2.20</t>
+  </si>
+  <si>
+    <t>2.59</t>
+  </si>
+  <si>
+    <t>4.60</t>
+  </si>
+  <si>
+    <t>4.31</t>
+  </si>
+  <si>
+    <t>2.75</t>
+  </si>
+  <si>
+    <t>4.15</t>
+  </si>
+  <si>
+    <t>4.80</t>
+  </si>
+  <si>
+    <t>3.00</t>
+  </si>
+  <si>
+    <t>2.10</t>
+  </si>
+  <si>
+    <t>3.91</t>
+  </si>
+  <si>
+    <t>2.90</t>
+  </si>
+  <si>
+    <t>3.50</t>
+  </si>
+  <si>
+    <t>3.58</t>
+  </si>
+  <si>
+    <t>2.88</t>
+  </si>
+  <si>
+    <t>2.98</t>
+  </si>
+  <si>
+    <t>30.7</t>
+  </si>
+  <si>
+    <t>34.9</t>
+  </si>
+  <si>
+    <t>39.6</t>
+  </si>
+  <si>
+    <t>43.0</t>
+  </si>
+  <si>
+    <t>28.3</t>
+  </si>
+  <si>
+    <t>39.2</t>
+  </si>
+  <si>
+    <t>1.64</t>
+  </si>
+  <si>
+    <t>4.53</t>
+  </si>
+  <si>
+    <t>2.65</t>
+  </si>
+  <si>
+    <t>4.23</t>
+  </si>
+  <si>
+    <t>2.89</t>
+  </si>
+  <si>
+    <t>3.46</t>
+  </si>
+  <si>
+    <t>2.97</t>
+  </si>
+  <si>
+    <t>4.26</t>
+  </si>
+  <si>
+    <t>3.31</t>
+  </si>
+  <si>
+    <t>3.42</t>
+  </si>
+  <si>
+    <t>3.09</t>
+  </si>
+  <si>
+    <t>29.4</t>
+  </si>
+  <si>
+    <t>40.2</t>
+  </si>
+  <si>
+    <t>31.3</t>
+  </si>
+  <si>
+    <t>43.8</t>
+  </si>
+  <si>
+    <t>28.4</t>
+  </si>
+  <si>
+    <t>37.6</t>
+  </si>
+  <si>
+    <t>38.6</t>
+  </si>
+  <si>
+    <t>35.3</t>
+  </si>
+  <si>
+    <t>31.1</t>
+  </si>
+  <si>
+    <t>1.38</t>
+  </si>
+  <si>
+    <t>4.75</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>3.41</t>
+  </si>
+  <si>
+    <t>2.17</t>
+  </si>
+  <si>
+    <t>4.35</t>
+  </si>
+  <si>
+    <t>4.88</t>
+  </si>
+  <si>
+    <t>4.25</t>
+  </si>
+  <si>
+    <t>4.72</t>
+  </si>
+  <si>
+    <t>3.54</t>
+  </si>
+  <si>
+    <t>3.06</t>
+  </si>
+  <si>
+    <t>2.84</t>
+  </si>
+  <si>
+    <t>2.86</t>
+  </si>
+  <si>
+    <t>3.98</t>
+  </si>
+  <si>
+    <t>4.39</t>
+  </si>
+  <si>
+    <t>4.89</t>
+  </si>
+  <si>
+    <t>5.68</t>
+  </si>
+  <si>
+    <t>2.76</t>
+  </si>
+  <si>
+    <t>29.9</t>
+  </si>
+  <si>
+    <t>36.6</t>
+  </si>
+  <si>
+    <t>34.2</t>
+  </si>
+  <si>
+    <t>28.6</t>
+  </si>
+  <si>
+    <t>1.77</t>
+  </si>
+  <si>
+    <t>5.41</t>
+  </si>
+  <si>
+    <t>5.83</t>
+  </si>
+  <si>
+    <t>6.69</t>
+  </si>
+  <si>
+    <t>4.70</t>
+  </si>
+  <si>
+    <t>5.26</t>
+  </si>
+  <si>
+    <t>3.84</t>
+  </si>
+  <si>
+    <t>4.08</t>
+  </si>
+  <si>
+    <t>3.87</t>
+  </si>
+  <si>
+    <t>3.34</t>
+  </si>
+  <si>
+    <t>41.7</t>
+  </si>
+  <si>
+    <t>39.7</t>
+  </si>
+  <si>
+    <t>30.9</t>
+  </si>
+  <si>
+    <t>28.8</t>
   </si>
 </sst>
 </file>
@@ -1273,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A0FBC84-188C-44FD-BCFB-366D6596A710}">
   <dimension ref="A1:AM25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="AC5" workbookViewId="0">
+      <selection activeCell="AK25" sqref="AK25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1471,19 +1720,37 @@
       <c r="X2" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="Y2" s="1"/>
+      <c r="Y2" s="1" t="s">
+        <v>284</v>
+      </c>
       <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
+      <c r="AA2" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>319</v>
+      </c>
       <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
+      <c r="AD2" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>336</v>
+      </c>
       <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
+      <c r="AG2" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>363</v>
+      </c>
       <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
+      <c r="AJ2" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="AL2" s="1"/>
       <c r="AM2" s="1"/>
     </row>
@@ -1556,19 +1823,37 @@
       <c r="X3" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="Y3" s="1"/>
+      <c r="Y3" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
+      <c r="AA3" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
+      <c r="AD3" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
+      <c r="AG3" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>282</v>
+      </c>
       <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
+      <c r="AJ3" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
     </row>
@@ -1641,19 +1926,37 @@
       <c r="X4" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="Y4" s="1"/>
+      <c r="Y4" s="1" t="s">
+        <v>281</v>
+      </c>
       <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
+      <c r="AA4" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
+      <c r="AD4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
+      <c r="AG4" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
+      <c r="AJ4" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>377</v>
+      </c>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
     </row>
@@ -1726,19 +2029,37 @@
       <c r="X5" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="Y5" s="1"/>
+      <c r="Y5" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
+      <c r="AA5" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
+      <c r="AD5" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
+      <c r="AG5" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1"/>
+      <c r="AJ5" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
     </row>
@@ -1811,19 +2132,37 @@
       <c r="X6" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="Y6" s="1"/>
+      <c r="Y6" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
+      <c r="AA6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>140</v>
+      </c>
       <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
+      <c r="AD6" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>185</v>
+      </c>
       <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
+      <c r="AG6" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="AH6" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
+      <c r="AJ6" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="AL6" s="1"/>
       <c r="AM6" s="1"/>
     </row>
@@ -1896,19 +2235,37 @@
       <c r="X7" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="Y7" s="1"/>
+      <c r="Y7" s="1" t="s">
+        <v>298</v>
+      </c>
       <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
+      <c r="AA7" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="AB7" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
+      <c r="AD7" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="AE7" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
+      <c r="AG7" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>216</v>
+      </c>
       <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-      <c r="AK7" s="1"/>
+      <c r="AJ7" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="AL7" s="1"/>
       <c r="AM7" s="1"/>
     </row>
@@ -1981,19 +2338,37 @@
       <c r="X8" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="Y8" s="1"/>
+      <c r="Y8" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
+      <c r="AA8" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="AB8" s="1" t="s">
+        <v>321</v>
+      </c>
       <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
+      <c r="AD8" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="AE8" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
+      <c r="AG8" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>337</v>
+      </c>
       <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
-      <c r="AK8" s="1"/>
+      <c r="AJ8" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="AL8" s="1"/>
       <c r="AM8" s="1"/>
     </row>
@@ -2066,19 +2441,37 @@
       <c r="X9" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="Y9" s="1"/>
+      <c r="Y9" s="1" t="s">
+        <v>301</v>
+      </c>
       <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
+      <c r="AA9" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
+      <c r="AD9" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="AE9" s="1" t="s">
+        <v>339</v>
+      </c>
       <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
+      <c r="AG9" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
+      <c r="AJ9" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="AL9" s="1"/>
       <c r="AM9" s="1"/>
     </row>
@@ -2151,19 +2544,37 @@
       <c r="X10" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="Y10" s="1"/>
+      <c r="Y10" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
+      <c r="AA10" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="AB10" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
+      <c r="AD10" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="AE10" s="1" t="s">
+        <v>210</v>
+      </c>
       <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
+      <c r="AG10" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="AH10" s="1" t="s">
+        <v>212</v>
+      </c>
       <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
+      <c r="AJ10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>378</v>
+      </c>
       <c r="AL10" s="1"/>
       <c r="AM10" s="1"/>
     </row>
@@ -2236,19 +2647,37 @@
       <c r="X11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Y11" s="1"/>
+      <c r="Y11" s="1" t="s">
+        <v>284</v>
+      </c>
       <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
+      <c r="AA11" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
+      <c r="AD11" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="AE11" s="1" t="s">
+        <v>226</v>
+      </c>
       <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
+      <c r="AG11" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH11" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1"/>
+      <c r="AJ11" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>188</v>
+      </c>
       <c r="AL11" s="1"/>
       <c r="AM11" s="1"/>
     </row>
@@ -2321,19 +2750,37 @@
       <c r="X12" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Y12" s="1"/>
+      <c r="Y12" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
+      <c r="AA12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>150</v>
+      </c>
       <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
-      <c r="AE12" s="1"/>
+      <c r="AD12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE12" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="AF12" s="1"/>
-      <c r="AG12" s="1"/>
-      <c r="AH12" s="1"/>
+      <c r="AG12" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="AH12" s="1" t="s">
+        <v>338</v>
+      </c>
       <c r="AI12" s="1"/>
-      <c r="AJ12" s="1"/>
-      <c r="AK12" s="1"/>
+      <c r="AJ12" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>379</v>
+      </c>
       <c r="AL12" s="1"/>
       <c r="AM12" s="1"/>
     </row>
@@ -2406,19 +2853,37 @@
       <c r="X13" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="Y13" s="1"/>
+      <c r="Y13" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
+      <c r="AA13" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
-      <c r="AE13" s="1"/>
+      <c r="AD13" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>340</v>
+      </c>
       <c r="AF13" s="1"/>
-      <c r="AG13" s="1"/>
-      <c r="AH13" s="1"/>
+      <c r="AG13" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="AH13" s="1" t="s">
+        <v>366</v>
+      </c>
       <c r="AI13" s="1"/>
-      <c r="AJ13" s="1"/>
-      <c r="AK13" s="1"/>
+      <c r="AJ13" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>285</v>
+      </c>
       <c r="AL13" s="1"/>
       <c r="AM13" s="1"/>
     </row>
@@ -2491,19 +2956,37 @@
       <c r="X14" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="Y14" s="1"/>
+      <c r="Y14" s="1" t="s">
+        <v>228</v>
+      </c>
       <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
+      <c r="AA14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
-      <c r="AE14" s="1"/>
+      <c r="AD14" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="AF14" s="1"/>
-      <c r="AG14" s="1"/>
-      <c r="AH14" s="1"/>
+      <c r="AG14" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="AI14" s="1"/>
-      <c r="AJ14" s="1"/>
-      <c r="AK14" s="1"/>
+      <c r="AJ14" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="AK14" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="AL14" s="1"/>
       <c r="AM14" s="1"/>
     </row>
@@ -2576,19 +3059,37 @@
       <c r="X15" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="Y15" s="1"/>
+      <c r="Y15" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
+      <c r="AA15" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>300</v>
+      </c>
       <c r="AC15" s="1"/>
-      <c r="AD15" s="1"/>
-      <c r="AE15" s="1"/>
+      <c r="AD15" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>342</v>
+      </c>
       <c r="AF15" s="1"/>
-      <c r="AG15" s="1"/>
-      <c r="AH15" s="1"/>
+      <c r="AG15" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="AH15" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="AI15" s="1"/>
-      <c r="AJ15" s="1"/>
-      <c r="AK15" s="1"/>
+      <c r="AJ15" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="AK15" s="1" t="s">
+        <v>208</v>
+      </c>
       <c r="AL15" s="1"/>
       <c r="AM15" s="1"/>
     </row>
@@ -2661,19 +3162,37 @@
       <c r="X16" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="Y16" s="1"/>
+      <c r="Y16" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
+      <c r="AA16" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>213</v>
+      </c>
       <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="1"/>
+      <c r="AD16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="AF16" s="1"/>
-      <c r="AG16" s="1"/>
-      <c r="AH16" s="1"/>
+      <c r="AG16" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AH16" s="1" t="s">
+        <v>114</v>
+      </c>
       <c r="AI16" s="1"/>
-      <c r="AJ16" s="1"/>
-      <c r="AK16" s="1"/>
+      <c r="AJ16" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>337</v>
+      </c>
       <c r="AL16" s="1"/>
       <c r="AM16" s="1"/>
     </row>
@@ -2746,19 +3265,37 @@
       <c r="X17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="Y17" s="1"/>
+      <c r="Y17" s="1" t="s">
+        <v>302</v>
+      </c>
       <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
+      <c r="AA17" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="AB17" s="1" t="s">
+        <v>287</v>
+      </c>
       <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
-      <c r="AE17" s="1"/>
+      <c r="AD17" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="AF17" s="1"/>
-      <c r="AG17" s="1"/>
-      <c r="AH17" s="1"/>
+      <c r="AG17" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="AH17" s="1" t="s">
+        <v>364</v>
+      </c>
       <c r="AI17" s="1"/>
-      <c r="AJ17" s="1"/>
-      <c r="AK17" s="1"/>
+      <c r="AJ17" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="AK17" s="1" t="s">
+        <v>207</v>
+      </c>
       <c r="AL17" s="1"/>
       <c r="AM17" s="1"/>
     </row>
@@ -2831,19 +3368,37 @@
       <c r="X18" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="Y18" s="1"/>
+      <c r="Y18" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
+      <c r="AA18" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
-      <c r="AE18" s="1"/>
+      <c r="AD18" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>343</v>
+      </c>
       <c r="AF18" s="1"/>
-      <c r="AG18" s="1"/>
-      <c r="AH18" s="1"/>
+      <c r="AG18" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="AH18" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="AI18" s="1"/>
-      <c r="AJ18" s="1"/>
-      <c r="AK18" s="1"/>
+      <c r="AJ18" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AK18" s="1" t="s">
+        <v>287</v>
+      </c>
       <c r="AL18" s="1"/>
       <c r="AM18" s="1"/>
     </row>
@@ -2916,19 +3471,37 @@
       <c r="X19" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="Y19" s="1"/>
+      <c r="Y19" s="1" t="s">
+        <v>191</v>
+      </c>
       <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
+      <c r="AA19" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-      <c r="AE19" s="1"/>
+      <c r="AD19" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="AE19" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="AF19" s="1"/>
-      <c r="AG19" s="1"/>
-      <c r="AH19" s="1"/>
+      <c r="AG19" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AH19" s="1" t="s">
+        <v>365</v>
+      </c>
       <c r="AI19" s="1"/>
-      <c r="AJ19" s="1"/>
-      <c r="AK19" s="1"/>
+      <c r="AJ19" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="AK19" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="AL19" s="1"/>
       <c r="AM19" s="1"/>
     </row>
@@ -3001,19 +3574,37 @@
       <c r="X20" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="Y20" s="1"/>
+      <c r="Y20" s="1" t="s">
+        <v>141</v>
+      </c>
       <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
+      <c r="AA20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB20" s="1" t="s">
+        <v>324</v>
+      </c>
       <c r="AC20" s="1"/>
-      <c r="AD20" s="1"/>
-      <c r="AE20" s="1"/>
+      <c r="AD20" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>283</v>
+      </c>
       <c r="AF20" s="1"/>
-      <c r="AG20" s="1"/>
-      <c r="AH20" s="1"/>
+      <c r="AG20" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="AH20" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="AI20" s="1"/>
-      <c r="AJ20" s="1"/>
-      <c r="AK20" s="1"/>
+      <c r="AJ20" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="AK20" s="1" t="s">
+        <v>190</v>
+      </c>
       <c r="AL20" s="1"/>
       <c r="AM20" s="1"/>
     </row>
@@ -3086,19 +3677,37 @@
       <c r="X21" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="Y21" s="1"/>
+      <c r="Y21" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
+      <c r="AA21" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
-      <c r="AE21" s="1"/>
+      <c r="AD21" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="AE21" s="1" t="s">
+        <v>193</v>
+      </c>
       <c r="AF21" s="1"/>
-      <c r="AG21" s="1"/>
-      <c r="AH21" s="1"/>
+      <c r="AG21" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="AH21" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="AI21" s="1"/>
-      <c r="AJ21" s="1"/>
-      <c r="AK21" s="1"/>
+      <c r="AJ21" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="AK21" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="AL21" s="1"/>
       <c r="AM21" s="1"/>
     </row>
@@ -3171,19 +3780,37 @@
       <c r="X22" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="Y22" s="1"/>
+      <c r="Y22" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-      <c r="AB22" s="1"/>
+      <c r="AA22" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="AB22" s="1" t="s">
+        <v>209</v>
+      </c>
       <c r="AC22" s="1"/>
-      <c r="AD22" s="1"/>
-      <c r="AE22" s="1"/>
+      <c r="AD22" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="AE22" s="1" t="s">
+        <v>344</v>
+      </c>
       <c r="AF22" s="1"/>
-      <c r="AG22" s="1"/>
-      <c r="AH22" s="1"/>
+      <c r="AG22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH22" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="AI22" s="1"/>
-      <c r="AJ22" s="1"/>
-      <c r="AK22" s="1"/>
+      <c r="AJ22" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="AK22" s="1" t="s">
+        <v>380</v>
+      </c>
       <c r="AL22" s="1"/>
       <c r="AM22" s="1"/>
     </row>
@@ -3256,19 +3883,37 @@
       <c r="X23" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="Y23" s="1"/>
+      <c r="Y23" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-      <c r="AB23" s="1"/>
+      <c r="AA23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>131</v>
+      </c>
       <c r="AC23" s="1"/>
-      <c r="AD23" s="1"/>
-      <c r="AE23" s="1"/>
+      <c r="AD23" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AE23" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="AF23" s="1"/>
-      <c r="AG23" s="1"/>
-      <c r="AH23" s="1"/>
+      <c r="AG23" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AH23" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="AI23" s="1"/>
-      <c r="AJ23" s="1"/>
-      <c r="AK23" s="1"/>
+      <c r="AJ23" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="AK23" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="AL23" s="1"/>
       <c r="AM23" s="1"/>
     </row>
@@ -3341,19 +3986,37 @@
       <c r="X24" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="Y24" s="1"/>
+      <c r="Y24" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
-      <c r="AB24" s="1"/>
+      <c r="AA24" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="AC24" s="1"/>
-      <c r="AD24" s="1"/>
-      <c r="AE24" s="1"/>
+      <c r="AD24" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="AE24" s="1" t="s">
+        <v>154</v>
+      </c>
       <c r="AF24" s="1"/>
-      <c r="AG24" s="1"/>
-      <c r="AH24" s="1"/>
+      <c r="AG24" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="AH24" s="1" t="s">
+        <v>302</v>
+      </c>
       <c r="AI24" s="1"/>
-      <c r="AJ24" s="1"/>
-      <c r="AK24" s="1"/>
+      <c r="AJ24" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="AK24" s="1" t="s">
+        <v>122</v>
+      </c>
       <c r="AL24" s="1"/>
       <c r="AM24" s="1"/>
     </row>

</xml_diff>